<commit_message>
TEST: Update test csv files to add campus
</commit_message>
<xml_diff>
--- a/test_files/csv_test_files/COS10001-Students.xlsx
+++ b/test_files/csv_test_files/COS10001-Students.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10310"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keshavkatarya/doubtfire-api/test_files/csv_test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caina/Documents/Code/GitHub/doubtfire-api/test_files/csv_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0565DA5-DC2C-E744-BCA0-382E8144D8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194F3BF2-A01E-3C45-BD87-862713A82CF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COS10001-Students" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>unit_code</t>
   </si>
@@ -59,13 +59,19 @@
   </si>
   <si>
     <t>test_csv_student</t>
+  </si>
+  <si>
+    <t>campus</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -909,16 +915,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,8 +946,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -959,11 +968,14 @@
       </c>
       <c r="G2" t="s">
         <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>